<commit_message>
COMPLETE: start to train 500 parameters
</commit_message>
<xml_diff>
--- a/Orange/result.xlsx
+++ b/Orange/result.xlsx
@@ -498,7 +498,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -507,29 +507,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>model_10</t>
+          <t>model_3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ModelType.SVR</t>
+          <t>ModelType.LINEAR_REGRESSION</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ScalerType.Normalizer_</t>
+          <t>ScalerType.MinMaxScaler_</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.3093889192968056</v>
+        <v>0.3290896630758111</v>
       </c>
       <c r="G3" t="n">
-        <v>1.266602510836622</v>
+        <v>1.230470725186108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -538,12 +538,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>model_8</t>
+          <t>model_2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ModelType.SVR</t>
+          <t>ModelType.LINEAR_REGRESSION</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -552,15 +552,15 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.2838011457834239</v>
+        <v>0.329089663075811</v>
       </c>
       <c r="G4" t="n">
-        <v>1.313531294756173</v>
+        <v>1.230470725186108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>model_4</t>
+          <t>model_6</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -579,19 +579,19 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ScalerType.Normalizer_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.2773614272766524</v>
+        <v>0.3290896630758109</v>
       </c>
       <c r="G5" t="n">
-        <v>1.325341941671152</v>
+        <v>1.230470725186108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -600,29 +600,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>model_25</t>
+          <t>model_5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.LINEAR_REGRESSION</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ScalerType.Raw_</t>
+          <t>ScalerType.RobustScaler_</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.2547040168462451</v>
+        <v>0.3290896630758104</v>
       </c>
       <c r="G6" t="n">
-        <v>1.366896347243373</v>
+        <v>1.230470725186109</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -631,12 +631,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>model_28</t>
+          <t>model_10</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.SVR</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -645,15 +645,15 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.2117387969965522</v>
+        <v>0.3093889192968056</v>
       </c>
       <c r="G7" t="n">
-        <v>1.445695916003343</v>
+        <v>1.266602510836622</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>model_7</t>
+          <t>model_8</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -672,19 +672,19 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ScalerType.Raw_</t>
+          <t>ScalerType.MaxAbsScaler_</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.2068601848948719</v>
+        <v>0.2950808275515512</v>
       </c>
       <c r="G8" t="n">
-        <v>1.454643444518371</v>
+        <v>1.292844002518694</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -693,29 +693,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>model_6</t>
+          <t>model_9</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ModelType.LINEAR_REGRESSION</t>
+          <t>ModelType.SVR</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.MinMaxScaler_</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.1539939845459654</v>
+        <v>0.2868884014121623</v>
       </c>
       <c r="G9" t="n">
-        <v>1.551601723890512</v>
+        <v>1.30786917052994</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -724,29 +724,29 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>model_11</t>
+          <t>model_4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ModelType.SVR</t>
+          <t>ModelType.LINEAR_REGRESSION</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ScalerType.RobustScaler_</t>
+          <t>ScalerType.Normalizer_</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.1466487340591264</v>
+        <v>0.2773614272766524</v>
       </c>
       <c r="G10" t="n">
-        <v>1.565073145026532</v>
+        <v>1.325341941671152</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -755,29 +755,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>model_5</t>
+          <t>model_12</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ModelType.LINEAR_REGRESSION</t>
+          <t>ModelType.SVR</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ScalerType.RobustScaler_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.1412898854836181</v>
+        <v>0.2771349193994743</v>
       </c>
       <c r="G11" t="n">
-        <v>1.574901442386054</v>
+        <v>1.325757364264236</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -786,7 +786,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>model_12</t>
+          <t>model_11</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -796,19 +796,19 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.RobustScaler_</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.1152525078755088</v>
+        <v>0.2740432104482925</v>
       </c>
       <c r="G12" t="n">
-        <v>1.622654814400376</v>
+        <v>1.331427656024333</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -817,29 +817,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>model_23</t>
+          <t>model_25</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ModelType.RANDOM_FOREST</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ScalerType.RobustScaler_</t>
+          <t>ScalerType.Raw_</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.09502468270594999</v>
+        <v>0.2547040168462451</v>
       </c>
       <c r="G13" t="n">
-        <v>1.659753283950618</v>
+        <v>1.366896347243373</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -848,29 +848,29 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>model_9</t>
+          <t>model_26</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ModelType.SVR</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ScalerType.MinMaxScaler_</t>
+          <t>ScalerType.MaxAbsScaler_</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.03943527734698271</v>
+        <v>0.2547040168462451</v>
       </c>
       <c r="G14" t="n">
-        <v>1.761706007228516</v>
+        <v>1.366896347243373</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -879,29 +879,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>model_2</t>
+          <t>model_27</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ModelType.LINEAR_REGRESSION</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ScalerType.MaxAbsScaler_</t>
+          <t>ScalerType.MinMaxScaler_</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.03554316709165317</v>
+        <v>0.2547040168462451</v>
       </c>
       <c r="G15" t="n">
-        <v>1.768844260233136</v>
+        <v>1.366896347243373</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -910,29 +910,29 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>model_22</t>
+          <t>model_30</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ModelType.RANDOM_FOREST</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ScalerType.Normalizer_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.02594136361285115</v>
+        <v>0.2545472350692494</v>
       </c>
       <c r="G16" t="n">
-        <v>1.786454270750817</v>
+        <v>1.367183889968859</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -941,29 +941,29 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>model_19</t>
+          <t>model_29</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ModelType.RANDOM_FOREST</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ScalerType.Raw_</t>
+          <t>ScalerType.RobustScaler_</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.01537899372405094</v>
+        <v>0.2529761818887426</v>
       </c>
       <c r="G17" t="n">
-        <v>1.805825990370371</v>
+        <v>1.370065251068744</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -972,29 +972,29 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>model_24</t>
+          <t>model_28</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ModelType.RANDOM_FOREST</t>
+          <t>ModelType.LIGHT_GBM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.Normalizer_</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.002177639043566493</v>
+        <v>0.2117387969965522</v>
       </c>
       <c r="G18" t="n">
-        <v>1.830037691358025</v>
+        <v>1.445695916003343</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1003,29 +1003,29 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>model_30</t>
+          <t>model_7</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.SVR</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.Raw_</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>-0.01509719290640588</v>
+        <v>0.2068601848948719</v>
       </c>
       <c r="G19" t="n">
-        <v>1.861720278176407</v>
+        <v>1.454643444518371</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1034,29 +1034,29 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>model_29</t>
+          <t>model_19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.RANDOM_FOREST</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>ScalerType.RobustScaler_</t>
+          <t>ScalerType.Raw_</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>-0.02088823986653909</v>
+        <v>0.0414956300501762</v>
       </c>
       <c r="G20" t="n">
-        <v>1.87234124100922</v>
+        <v>1.75792725536659</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1065,29 +1065,29 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>model_34</t>
+          <t>model_23</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ModelType.XGB</t>
+          <t>ModelType.RANDOM_FOREST</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ScalerType.Normalizer_</t>
+          <t>ScalerType.RobustScaler_</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>-0.02299239389664787</v>
+        <v>0.02172418665476583</v>
       </c>
       <c r="G21" t="n">
-        <v>1.876200325886644</v>
+        <v>1.794188706344167</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1096,29 +1096,29 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>model_35</t>
+          <t>model_24</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ModelType.XGB</t>
+          <t>ModelType.RANDOM_FOREST</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ScalerType.RobustScaler_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>-0.03739776102070813</v>
+        <v>0.01921383028087453</v>
       </c>
       <c r="G22" t="n">
-        <v>1.902620223682491</v>
+        <v>1.7987927791358</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>model_20</t>
+          <t>model_21</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1137,19 +1137,19 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ScalerType.MaxAbsScaler_</t>
+          <t>ScalerType.MinMaxScaler_</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>-0.03970176154386129</v>
+        <v>-0.004560913666249888</v>
       </c>
       <c r="G23" t="n">
-        <v>1.906845833333328</v>
+        <v>1.842396409629628</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1158,29 +1158,29 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>model_36</t>
+          <t>model_20</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ModelType.XGB</t>
+          <t>ModelType.RANDOM_FOREST</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.MaxAbsScaler_</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>-0.09808515477349489</v>
+        <v>-0.008149507841756609</v>
       </c>
       <c r="G24" t="n">
-        <v>2.013922818516537</v>
+        <v>1.8489780045679</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1189,29 +1189,29 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>model_31</t>
+          <t>model_22</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ModelType.XGB</t>
+          <t>ModelType.RANDOM_FOREST</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ScalerType.Raw_</t>
+          <t>ScalerType.Normalizer_</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>-0.1331679466264639</v>
+        <v>-0.01716134449921425</v>
       </c>
       <c r="G25" t="n">
-        <v>2.078265765639371</v>
+        <v>1.865505997321742</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1220,29 +1220,29 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>model_26</t>
+          <t>model_34</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.XGB</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ScalerType.MaxAbsScaler_</t>
+          <t>ScalerType.Normalizer_</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>-0.1977578642412463</v>
+        <v>-0.02299239389664787</v>
       </c>
       <c r="G26" t="n">
-        <v>2.196725712361213</v>
+        <v>1.876200325886644</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>model_32</t>
+          <t>model_31</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1261,19 +1261,19 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ScalerType.MaxAbsScaler_</t>
+          <t>ScalerType.Raw_</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>-0.2768825240115735</v>
+        <v>-0.1331679466264639</v>
       </c>
       <c r="G27" t="n">
-        <v>2.341842834768436</v>
+        <v>2.078265765639371</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1282,29 +1282,29 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>model_3</t>
+          <t>model_32</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ModelType.LINEAR_REGRESSION</t>
+          <t>ModelType.XGB</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>ScalerType.MinMaxScaler_</t>
+          <t>ScalerType.MaxAbsScaler_</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>-0.3015585906687679</v>
+        <v>-0.1331679466264639</v>
       </c>
       <c r="G28" t="n">
-        <v>2.387099519549326</v>
+        <v>2.078265765639371</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1313,29 +1313,29 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>model_14</t>
+          <t>model_33</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ModelType.DECISION_TREE</t>
+          <t>ModelType.XGB</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ScalerType.MaxAbsScaler_</t>
+          <t>ScalerType.MinMaxScaler_</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>-0.4929708027395479</v>
+        <v>-0.1331679466264639</v>
       </c>
       <c r="G29" t="n">
-        <v>2.738155555555556</v>
+        <v>2.078265765639371</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1344,29 +1344,29 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>model_27</t>
+          <t>model_35</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ModelType.LIGHT_GBM</t>
+          <t>ModelType.XGB</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>ScalerType.MinMaxScaler_</t>
+          <t>ScalerType.RobustScaler_</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>-0.5213867668702854</v>
+        <v>-0.1331679466264639</v>
       </c>
       <c r="G30" t="n">
-        <v>2.790271330296946</v>
+        <v>2.078265765639371</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1375,29 +1375,29 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>model_16</t>
+          <t>model_36</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ModelType.DECISION_TREE</t>
+          <t>ModelType.XGB</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ScalerType.Normalizer_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>-0.5815337069533564</v>
+        <v>-0.1331679466264639</v>
       </c>
       <c r="G31" t="n">
-        <v>2.900582716049383</v>
+        <v>2.078265765639371</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>model_13</t>
+          <t>model_16</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1416,19 +1416,19 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ScalerType.Raw_</t>
+          <t>ScalerType.Normalizer_</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>-0.6670896755369637</v>
+        <v>-0.5815337069533564</v>
       </c>
       <c r="G32" t="n">
-        <v>3.057495061728396</v>
+        <v>2.900582716049383</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1437,12 +1437,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>model_21</t>
+          <t>model_15</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ModelType.RANDOM_FOREST</t>
+          <t>ModelType.DECISION_TREE</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1451,15 +1451,15 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>-0.7003496346247289</v>
+        <v>-0.6487801503206039</v>
       </c>
       <c r="G33" t="n">
-        <v>3.118494876049347</v>
+        <v>3.023914814814815</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>model_18</t>
+          <t>model_13</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1478,14 +1478,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>ScalerType.StandardScaler_</t>
+          <t>ScalerType.Raw_</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>-1.185074221639495</v>
+        <v>-0.6670896755369637</v>
       </c>
       <c r="G34" t="n">
-        <v>4.007495061728395</v>
+        <v>3.057495061728396</v>
       </c>
     </row>
     <row r="35">
@@ -1513,15 +1513,15 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>-1.228424715166465</v>
+        <v>-0.6670896755369637</v>
       </c>
       <c r="G35" t="n">
-        <v>4.087001234567901</v>
+        <v>3.057495061728396</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1530,29 +1530,29 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>model_33</t>
+          <t>model_18</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ModelType.XGB</t>
+          <t>ModelType.DECISION_TREE</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ScalerType.MinMaxScaler_</t>
+          <t>ScalerType.StandardScaler_</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>-1.278920114725987</v>
+        <v>-0.6688398507414688</v>
       </c>
       <c r="G36" t="n">
-        <v>4.179611390493384</v>
+        <v>3.060704938271605</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>model_15</t>
+          <t>model_14</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1571,14 +1571,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>ScalerType.MinMaxScaler_</t>
+          <t>ScalerType.MaxAbsScaler_</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>-1.454291556750928</v>
+        <v>-0.6727440877361337</v>
       </c>
       <c r="G37" t="n">
-        <v>4.501248148148151</v>
+        <v>3.067865432098765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>